<commit_message>
Push code check attandance
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,10 +711,8 @@
           <t>Poleak Theng</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B10" t="n">
+        <v>20</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -734,6 +732,38 @@
       <c r="F10" t="inlineStr">
         <is>
           <t>image\fcfb0d6ff97147a7aa7ad3cff77c06c8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sina Neak</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Kompot</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Class B 2025</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>image\34e67118c6594bcd88ac6902475643c7.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
push code to main
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -741,29 +741,239 @@
           <t>Sina Neak</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>21</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Kompot</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Class B 2025</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>image\34e67118c6594bcd88ac6902475643c7.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Solin Neat</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>22</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Kompong Thom</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Class B 2025</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>image\55b8f49f301c47a6b7ee3000cc00bcbe.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Bopha Khat</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>20</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kompot</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Class B 2025</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>image\fcfd397106ad4bbdbb133df0246a792d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bunyoung Hean</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>23</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Rotanakiri</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Class A 2025</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>image\778c5d5c26024057a335cd35381b9996.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Chhun Kimchhik</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bathombong</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Class A 2025</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>image\da72b4ddf65e47a8b18eaa5e866879c5.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Kanha Mao</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Priveng </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Class B 2025</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>image\ea1715a1a8354986b29cc68c6c0224d8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Channak Kan</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bathombong </t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Class B 2025</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>image\ece17cec0596494f9747286afaab640d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Hort Heng</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Kompot</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Class B 2025</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>image\34e67118c6594bcd88ac6902475643c7.png</t>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Priveng</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Class A 2025</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>image\0909ecf105fe4905a3a7d5816b1bbc3b.png</t>
         </is>
       </c>
     </row>

</xml_diff>